<commit_message>
P21 et P22, CSV seulement
</commit_message>
<xml_diff>
--- a/Saison22/DonnéesCSV/Saisie des points.xlsx
+++ b/Saison22/DonnéesCSV/Saisie des points.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siromar\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siromar\Documents\Github\gehstatcan.github.io\Saison22\DonnéesCSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47221D1-D388-4769-A835-1E9016A80481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2591EECF-29F7-4098-BC41-C06DE1DF147F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -678,10 +678,10 @@
   <autoFilter ref="A1:E9" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="NoÉquipe"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="NomÉquipe" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="PosFinale" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="NomÉquipe" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="PosFinale" dataDxfId="8"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Carillon"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="NoÉquipe2" dataDxfId="9">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="NoÉquipe2" dataDxfId="7">
       <calculatedColumnFormula>tblÉquipes[[#This Row],[NoÉquipe]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1015,7 +1015,7 @@
   <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,7 +1053,7 @@
         <v>138</v>
       </c>
       <c r="B2" s="3">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1061,11 +1061,11 @@
         <v>131</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <f>VLOOKUP(B3,tblÉquipes[[#All],[NomÉquipe]:[NoÉquipe2]],4,FALSE)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>139</v>
@@ -1085,64 +1085,64 @@
         <v>132</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <f>VLOOKUP(B4,tblÉquipes[[#All],[NomÉquipe]:[NoÉquipe2]],4,FALSE)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F4" cm="1">
         <f t="array" ref="F4:I13">_xlfn._xlws.FILTER(F18:I42,I18:I42&gt;0)</f>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
       <c r="I4">
-        <v>85</v>
+        <v>120</v>
       </c>
       <c r="K4" t="str">
         <f>F4&amp;","&amp;G4&amp;","&amp;H4&amp;","&amp;I4</f>
-        <v>19,5,1,85</v>
+        <v>22,7,1,120</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F5">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I5">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="K5" t="str">
         <f t="shared" ref="K5:K13" si="0">F5&amp;","&amp;G5&amp;","&amp;H5&amp;","&amp;I5</f>
-        <v>19,5,2,80</v>
+        <v>22,7,3,105</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F6">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G6">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I6">
-        <v>30</v>
+        <v>150</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="0"/>
-        <v>19,5,3,30</v>
+        <v>22,7,4,150</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1159,236 +1159,232 @@
         <v>137</v>
       </c>
       <c r="F7">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H7">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="I7">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="K7" t="str">
         <f t="shared" si="0"/>
-        <v>19,5,4,20</v>
+        <v>22,7,12,40</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" cm="1">
-        <f t="array" ref="A8:C28">_xlfn._xlws.FILTER(tblJoueurs!I:K,(tblJoueurs!I:I=$C$3)+(tblJoueurs!I:I=$C$4),"")</f>
-        <v>5</v>
+        <f t="array" ref="A8:C29">_xlfn._xlws.FILTER(tblJoueurs!I:K,(tblJoueurs!I:I=$C$3)+(tblJoueurs!I:I=$C$4),"")</f>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="str">
-        <v>Bruno Lapierre</v>
+        <v>Philippe Bérubé</v>
       </c>
       <c r="D8" s="3">
-        <v>85</v>
+        <v>120</v>
       </c>
       <c r="F8">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G8">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H8">
         <v>99</v>
       </c>
       <c r="I8">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="0"/>
-        <v>19,5,99,85</v>
+        <v>22,7,99,65</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9" t="str">
-        <v>Julie Bernier</v>
-      </c>
-      <c r="D9" s="3">
-        <v>80</v>
-      </c>
+        <v>Tony Labillois</v>
+      </c>
+      <c r="D9" s="3"/>
       <c r="F9">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I9">
-        <v>120</v>
+        <v>20</v>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="0"/>
-        <v>19,6,1,120</v>
+        <v>22,8,4,20</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B10">
         <v>3</v>
       </c>
       <c r="C10" t="str">
-        <v>Sylvain Perron</v>
+        <v>Éric Caron-Malenfant</v>
       </c>
       <c r="D10" s="3">
-        <v>30</v>
+        <v>105</v>
       </c>
       <c r="F10">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G10">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H10">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I10">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="0"/>
-        <v>19,6,2,60</v>
+        <v>22,8,5,80</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B11">
         <v>4</v>
       </c>
       <c r="C11" t="str">
-        <v>Martin Sirois</v>
+        <v>Pierre Galarneau</v>
       </c>
       <c r="D11" s="3">
-        <v>20</v>
+        <v>150</v>
       </c>
       <c r="F11">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G11">
+        <v>8</v>
+      </c>
+      <c r="H11">
         <v>6</v>
-      </c>
-      <c r="H11">
-        <v>3</v>
       </c>
       <c r="I11">
         <v>40</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" si="0"/>
-        <v>19,6,3,40</v>
+        <v>22,8,6,40</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B12">
         <v>5</v>
       </c>
       <c r="C12" t="str">
-        <v>Didier Garriguet</v>
+        <v>Félix Labrecque-Synnott</v>
       </c>
       <c r="D12" s="3"/>
       <c r="F12">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G12">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H12">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I12">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="K12" t="str">
         <f t="shared" si="0"/>
-        <v>19,6,4,120</v>
+        <v>22,8,8,40</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B13">
         <v>6</v>
       </c>
       <c r="C13" t="str">
-        <v>Jean-Sébastien Provencal</v>
+        <v>Danielle Turpin</v>
       </c>
       <c r="D13" s="3"/>
       <c r="F13">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G13">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H13">
         <v>99</v>
       </c>
       <c r="I13">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="K13" t="str">
         <f t="shared" si="0"/>
-        <v>19,6,99,25</v>
+        <v>22,8,99,35</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B14">
         <v>7</v>
       </c>
       <c r="C14" t="str">
-        <v>Absent Absent</v>
+        <v>James Falconer</v>
       </c>
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B15">
         <v>8</v>
       </c>
       <c r="C15" t="str">
-        <v>Marlène Savard</v>
+        <v>Absent Absent</v>
       </c>
       <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B16">
-        <v>99</v>
+        <v>9</v>
       </c>
       <c r="C16" t="str">
-        <v>NA Les Méthos précieux</v>
-      </c>
-      <c r="D16" s="3">
-        <v>85</v>
-      </c>
+        <v>Catherine NA</v>
+      </c>
+      <c r="D16" s="3"/>
       <c r="F16" s="6" t="s">
         <v>141</v>
       </c>
@@ -1397,17 +1393,15 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C17" t="str">
-        <v>Stéphane Mongeau</v>
-      </c>
-      <c r="D17" s="3">
-        <v>120</v>
-      </c>
+        <v>Louis NA</v>
+      </c>
+      <c r="D17" s="3"/>
       <c r="F17" s="2" t="s">
         <v>139</v>
       </c>
@@ -1423,24 +1417,22 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C18" t="str">
-        <v>Pierre-Olivier Julien</v>
-      </c>
-      <c r="D18" s="3">
-        <v>60</v>
-      </c>
+        <v>Étienne Lemyre (Faciles)</v>
+      </c>
+      <c r="D18" s="3"/>
       <c r="F18">
         <f>$B$2</f>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G18">
         <f t="shared" ref="G18:G38" si="1">A8</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H18">
         <f t="shared" ref="H18:H38" si="2">B8</f>
@@ -1448,29 +1440,29 @@
       </c>
       <c r="I18">
         <f t="shared" ref="I18:I38" si="3">D8</f>
-        <v>85</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C19" t="str">
-        <v>Julien Bérard-Chagnon</v>
+        <v>Élizabeth LeBlanc</v>
       </c>
       <c r="D19" s="3">
         <v>40</v>
       </c>
       <c r="F19">
         <f t="shared" ref="F19:F42" si="4">$B$2</f>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G19">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H19">
         <f t="shared" si="2"/>
@@ -1478,29 +1470,29 @@
       </c>
       <c r="I19">
         <f t="shared" si="3"/>
-        <v>80</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B20">
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="C20" t="str">
-        <v>Patrick Charbonneau</v>
+        <v>NA Les Faciles à cuire</v>
       </c>
       <c r="D20" s="3">
-        <v>120</v>
+        <v>65</v>
       </c>
       <c r="F20">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G20">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H20">
         <f t="shared" si="2"/>
@@ -1508,27 +1500,27 @@
       </c>
       <c r="I20">
         <f t="shared" si="3"/>
-        <v>30</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B21">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C21" t="str">
-        <v>Keven Bosa</v>
+        <v>Stéphanie Audet-Brazeau</v>
       </c>
       <c r="D21" s="3"/>
       <c r="F21">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G21">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H21">
         <f t="shared" si="2"/>
@@ -1536,27 +1528,27 @@
       </c>
       <c r="I21">
         <f t="shared" si="3"/>
-        <v>20</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B22">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C22" t="str">
-        <v>Étienne Rassart</v>
+        <v>Julia Colpron</v>
       </c>
       <c r="D22" s="3"/>
       <c r="F22">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G22">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H22">
         <f t="shared" si="2"/>
@@ -1569,22 +1561,22 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B23">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C23" t="str">
-        <v>Daphné Allard Gervais</v>
+        <v>Isabelle Gamache</v>
       </c>
       <c r="D23" s="3"/>
       <c r="F23">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G23">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H23">
         <f t="shared" si="2"/>
@@ -1597,22 +1589,24 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B24">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C24" t="str">
-        <v>Emy Bourdages</v>
-      </c>
-      <c r="D24" s="3"/>
+        <v>Catherine Lachance</v>
+      </c>
+      <c r="D24" s="3">
+        <v>20</v>
+      </c>
       <c r="F24">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G24">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H24">
         <f t="shared" si="2"/>
@@ -1625,22 +1619,24 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B25">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C25" t="str">
-        <v>David Binet</v>
-      </c>
-      <c r="D25" s="3"/>
+        <v>Francis Vilandré</v>
+      </c>
+      <c r="D25" s="3">
+        <v>80</v>
+      </c>
       <c r="F25">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G25">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H25">
         <f t="shared" si="2"/>
@@ -1653,103 +1649,116 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
+        <v>8</v>
+      </c>
+      <c r="B26">
         <v>6</v>
       </c>
-      <c r="B26">
-        <v>10</v>
-      </c>
       <c r="C26" t="str">
-        <v>Absent Absent</v>
-      </c>
-      <c r="D26" s="3"/>
+        <v>Julie Sarrazin</v>
+      </c>
+      <c r="D26" s="3">
+        <v>40</v>
+      </c>
       <c r="F26">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G26">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H26">
         <f t="shared" si="2"/>
-        <v>99</v>
+        <v>9</v>
       </c>
       <c r="I26">
         <f t="shared" si="3"/>
-        <v>85</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B27">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C27" t="str">
-        <v>François Sergerie</v>
+        <v>Absent Absent</v>
       </c>
       <c r="D27" s="3"/>
       <c r="F27">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G27">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H27">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I27">
         <f t="shared" si="3"/>
-        <v>120</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B28">
-        <v>99</v>
+        <v>8</v>
       </c>
       <c r="C28" t="str">
-        <v>NA Les 12e meilleurs</v>
+        <v>Émilie Fougères</v>
       </c>
       <c r="D28" s="3">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="F28">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G28">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H28">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="I28">
         <f t="shared" si="3"/>
-        <v>60</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D29" s="3"/>
+      <c r="A29">
+        <v>8</v>
+      </c>
+      <c r="B29">
+        <v>99</v>
+      </c>
+      <c r="C29" t="str">
+        <v>NA Les Génies de la traduction</v>
+      </c>
+      <c r="D29" s="3">
+        <v>35</v>
+      </c>
       <c r="F29">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G29">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H29">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="I29">
         <f t="shared" si="3"/>
@@ -1760,34 +1769,34 @@
       <c r="D30" s="3"/>
       <c r="F30">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G30">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H30">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="I30">
         <f t="shared" si="3"/>
-        <v>120</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D31" s="3"/>
       <c r="F31">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G31">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H31">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I31">
         <f t="shared" si="3"/>
@@ -1798,15 +1807,15 @@
       <c r="D32" s="3"/>
       <c r="F32">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G32">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H32">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I32">
         <f t="shared" si="3"/>
@@ -1816,15 +1825,15 @@
     <row r="33" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F33">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G33">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H33">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I33">
         <f t="shared" si="3"/>
@@ -1834,69 +1843,69 @@
     <row r="34" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F34">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G34">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H34">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I34">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F35">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G35">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H35">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I35">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F36">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G36">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H36">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="I36">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F37">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G37">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H37">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I37">
         <f t="shared" si="3"/>
@@ -1906,43 +1915,43 @@
     <row r="38" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F38">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G38">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H38">
         <f t="shared" si="2"/>
-        <v>99</v>
+        <v>8</v>
       </c>
       <c r="I38">
         <f t="shared" si="3"/>
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F39">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G39">
         <f t="shared" ref="G39:H39" si="5">A29</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H39">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="I39">
         <f t="shared" ref="I39:I42" si="6">D29</f>
-        <v>0</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F40">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G40">
         <f t="shared" ref="G40:H40" si="7">A30</f>
@@ -1960,7 +1969,7 @@
     <row r="41" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F41">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G41">
         <f t="shared" ref="G41:H41" si="8">A31</f>
@@ -1978,7 +1987,7 @@
     <row r="42" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F42">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G42">
         <f t="shared" ref="G42:H42" si="9">A32</f>

</xml_diff>

<commit_message>
P25 et P26 csv+htm
</commit_message>
<xml_diff>
--- a/Saison22/DonnéesCSV/Saisie des points.xlsx
+++ b/Saison22/DonnéesCSV/Saisie des points.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://054gc-my.sharepoint.com/personal/martin_sirois_statcan_gc_ca/Documents/01_Perso/GEHStatcan GIT/gehstatcan.github.io/Saison22/DonnéesCSV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{2591EECF-29F7-4098-BC41-C06DE1DF147F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D2BD09B-E48C-4CF2-BD03-997FC967FB14}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="13_ncr:1_{2591EECF-29F7-4098-BC41-C06DE1DF147F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC6CC458-9C83-44C6-9894-B613ABAC8F36}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1015,7 +1015,7 @@
   <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4:K13"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,7 +1053,7 @@
         <v>138</v>
       </c>
       <c r="B2" s="3">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1061,11 +1061,11 @@
         <v>131</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <f>VLOOKUP(B3,tblÉquipes[[#All],[NomÉquipe]:[NoÉquipe2]],4,FALSE)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>139</v>
@@ -1085,64 +1085,64 @@
         <v>132</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <f>VLOOKUP(B4,tblÉquipes[[#All],[NomÉquipe]:[NoÉquipe2]],4,FALSE)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F4" cm="1">
         <f t="array" ref="F4:I13">_xlfn._xlws.FILTER(F18:I42,I18:I42&gt;0)</f>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
       <c r="I4">
-        <v>160</v>
+        <v>125</v>
       </c>
       <c r="K4" t="str">
         <f>F4&amp;","&amp;G4&amp;","&amp;H4&amp;","&amp;I4</f>
-        <v>24,2,1,160</v>
+        <v>26,4,1,125</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F5">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H5">
         <v>2</v>
       </c>
       <c r="I5">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="K5" t="str">
         <f t="shared" ref="K5:K13" si="0">F5&amp;","&amp;G5&amp;","&amp;H5&amp;","&amp;I5</f>
-        <v>24,2,2,20</v>
+        <v>26,4,2,80</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F6">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I6">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="0"/>
-        <v>24,2,4,60</v>
+        <v>26,4,3,80</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1159,236 +1159,234 @@
         <v>137</v>
       </c>
       <c r="F7">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H7">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I7">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="K7" t="str">
         <f t="shared" si="0"/>
-        <v>24,2,7,10</v>
+        <v>26,4,4,85</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" cm="1">
         <f t="array" ref="A8:C26">_xlfn._xlws.FILTER(tblJoueurs!I:K,(tblJoueurs!I:I=$C$3)+(tblJoueurs!I:I=$C$4),"")</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="str">
-        <v>Steeve Boisvert</v>
+        <v>Sébastien Landry</v>
       </c>
       <c r="D8" s="3">
-        <v>160</v>
+        <v>125</v>
       </c>
       <c r="F8">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H8">
         <v>99</v>
       </c>
       <c r="I8">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="0"/>
-        <v>24,2,99,10</v>
+        <v>26,4,99,45</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9" t="str">
-        <v>Samuel Perreault</v>
+        <v>Frédéric Bédard</v>
       </c>
       <c r="D9" s="3">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="F9">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H9">
         <v>1</v>
       </c>
       <c r="I9">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="0"/>
-        <v>24,4,1,95</v>
+        <v>26,8,1,110</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B10">
         <v>3</v>
       </c>
       <c r="C10" t="str">
-        <v>Jonathan Baillargeon</v>
-      </c>
-      <c r="D10" s="3"/>
+        <v>Geneviève Ouellet</v>
+      </c>
+      <c r="D10" s="3">
+        <v>80</v>
+      </c>
       <c r="F10">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G10">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H10">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I10">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="0"/>
-        <v>24,4,2,90</v>
+        <v>26,8,5,105</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B11">
         <v>4</v>
       </c>
       <c r="C11" t="str">
-        <v>Vincent Hardy</v>
+        <v>Samuel Vézina</v>
       </c>
       <c r="D11" s="3">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="F11">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G11">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H11">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I11">
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" si="0"/>
-        <v>24,4,3,90</v>
+        <v>26,8,6,20</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B12">
         <v>5</v>
       </c>
       <c r="C12" t="str">
-        <v>Nicole Paquin</v>
+        <v>Jean-Dominique Morency</v>
       </c>
       <c r="D12" s="3"/>
       <c r="F12">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G12">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H12">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I12">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="K12" t="str">
         <f t="shared" si="0"/>
-        <v>24,4,4,60</v>
+        <v>26,8,8,20</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B13">
         <v>6</v>
       </c>
       <c r="C13" t="str">
-        <v>Franklin Assoumou</v>
+        <v>Stéphane Martineau</v>
       </c>
       <c r="D13" s="3"/>
       <c r="F13">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G13">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H13">
         <v>99</v>
       </c>
       <c r="I13">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="K13" t="str">
         <f t="shared" si="0"/>
-        <v>24,4,99,25</v>
+        <v>26,8,99,55</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B14">
         <v>7</v>
       </c>
       <c r="C14" t="str">
-        <v>Marie-Hélène Sarrasin</v>
-      </c>
-      <c r="D14" s="3">
-        <v>10</v>
-      </c>
+        <v>Michel Parenteau</v>
+      </c>
+      <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B15">
         <v>8</v>
       </c>
       <c r="C15" t="str">
-        <v>Absent Absent</v>
+        <v>Caroline Pelletier</v>
       </c>
       <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B16">
-        <v>99</v>
+        <v>9</v>
       </c>
       <c r="C16" t="str">
-        <v>NA Les Bons Perdants</v>
-      </c>
-      <c r="D16" s="3">
-        <v>10</v>
-      </c>
+        <v>Absent Absent</v>
+      </c>
+      <c r="D16" s="3"/>
       <c r="F16" s="6" t="s">
         <v>141</v>
       </c>
@@ -1400,13 +1398,13 @@
         <v>4</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>99</v>
       </c>
       <c r="C17" t="str">
-        <v>Sébastien Landry</v>
+        <v>NA Les Herbizarres</v>
       </c>
       <c r="D17" s="3">
-        <v>95</v>
+        <v>45</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>139</v>
@@ -1423,24 +1421,24 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18" t="str">
-        <v>Frédéric Bédard</v>
+        <v>Stéphanie Audet-Brazeau</v>
       </c>
       <c r="D18" s="3">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="F18">
         <f>$B$2</f>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G18">
         <f t="shared" ref="G18:G38" si="1">A8</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H18">
         <f t="shared" ref="H18:H38" si="2">B8</f>
@@ -1448,29 +1446,27 @@
       </c>
       <c r="I18">
         <f t="shared" ref="I18:I38" si="3">D8</f>
-        <v>160</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C19" t="str">
-        <v>Geneviève Ouellet</v>
-      </c>
-      <c r="D19" s="3">
-        <v>90</v>
-      </c>
+        <v>Julia Colpron</v>
+      </c>
+      <c r="D19" s="3"/>
       <c r="F19">
         <f t="shared" ref="F19:F42" si="4">$B$2</f>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G19">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H19">
         <f t="shared" si="2"/>
@@ -1478,29 +1474,27 @@
       </c>
       <c r="I19">
         <f t="shared" si="3"/>
-        <v>20</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C20" t="str">
-        <v>Samuel Vézina</v>
-      </c>
-      <c r="D20" s="3">
-        <v>60</v>
-      </c>
+        <v>Isabelle Gamache</v>
+      </c>
+      <c r="D20" s="3"/>
       <c r="F20">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G20">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H20">
         <f t="shared" si="2"/>
@@ -1508,27 +1502,27 @@
       </c>
       <c r="I20">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B21">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C21" t="str">
-        <v>Jean-Dominique Morency</v>
+        <v>Catherine Lachance</v>
       </c>
       <c r="D21" s="3"/>
       <c r="F21">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G21">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H21">
         <f t="shared" si="2"/>
@@ -1536,27 +1530,29 @@
       </c>
       <c r="I21">
         <f t="shared" si="3"/>
-        <v>60</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B22">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22" t="str">
-        <v>Stéphane Martineau</v>
-      </c>
-      <c r="D22" s="3"/>
+        <v>Francis Vilandré</v>
+      </c>
+      <c r="D22" s="3">
+        <v>105</v>
+      </c>
       <c r="F22">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G22">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H22">
         <f t="shared" si="2"/>
@@ -1569,22 +1565,24 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B23">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C23" t="str">
-        <v>Michel Parenteau</v>
-      </c>
-      <c r="D23" s="3"/>
+        <v>Julie Sarrazin</v>
+      </c>
+      <c r="D23" s="3">
+        <v>20</v>
+      </c>
       <c r="F23">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G23">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H23">
         <f t="shared" si="2"/>
@@ -1597,22 +1595,22 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B24">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C24" t="str">
-        <v>Caroline Pelletier</v>
+        <v>Absent Absent</v>
       </c>
       <c r="D24" s="3"/>
       <c r="F24">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G24">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H24">
         <f t="shared" si="2"/>
@@ -1620,27 +1618,29 @@
       </c>
       <c r="I24">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B25">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C25" t="str">
-        <v>Absent Absent</v>
-      </c>
-      <c r="D25" s="3"/>
+        <v>Émilie Fougères</v>
+      </c>
+      <c r="D25" s="3">
+        <v>20</v>
+      </c>
       <c r="F25">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G25">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H25">
         <f t="shared" si="2"/>
@@ -1653,39 +1653,39 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B26">
         <v>99</v>
       </c>
       <c r="C26" t="str">
-        <v>NA Les Herbizarres</v>
+        <v>NA Les Génies de la traduction</v>
       </c>
       <c r="D26" s="3">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="F26">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G26">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H26">
         <f t="shared" si="2"/>
-        <v>99</v>
+        <v>9</v>
       </c>
       <c r="I26">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D27" s="3"/>
       <c r="F27">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G27">
         <f t="shared" si="1"/>
@@ -1693,83 +1693,83 @@
       </c>
       <c r="H27">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>99</v>
       </c>
       <c r="I27">
         <f t="shared" si="3"/>
-        <v>95</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D28" s="3"/>
       <c r="F28">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G28">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H28">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I28">
         <f t="shared" si="3"/>
-        <v>90</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D29" s="3"/>
       <c r="F29">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G29">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H29">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I29">
         <f t="shared" si="3"/>
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D30" s="3"/>
       <c r="F30">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G30">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H30">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I30">
         <f t="shared" si="3"/>
-        <v>60</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D31" s="3"/>
       <c r="F31">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G31">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H31">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I31">
         <f t="shared" si="3"/>
@@ -1780,51 +1780,51 @@
       <c r="D32" s="3"/>
       <c r="F32">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G32">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H32">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I32">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F33">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G33">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H33">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I33">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F34">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G34">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H34">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I34">
         <f t="shared" si="3"/>
@@ -1834,29 +1834,29 @@
     <row r="35" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F35">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G35">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H35">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I35">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F36">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G36">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H36">
         <f t="shared" si="2"/>
@@ -1864,13 +1864,13 @@
       </c>
       <c r="I36">
         <f t="shared" si="3"/>
-        <v>25</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F37">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G37">
         <f t="shared" si="1"/>
@@ -1888,7 +1888,7 @@
     <row r="38" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F38">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G38">
         <f t="shared" si="1"/>
@@ -1906,7 +1906,7 @@
     <row r="39" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F39">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G39">
         <f t="shared" ref="G39:H39" si="5">A29</f>
@@ -1924,7 +1924,7 @@
     <row r="40" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F40">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G40">
         <f t="shared" ref="G40:H40" si="7">A30</f>
@@ -1942,7 +1942,7 @@
     <row r="41" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F41">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G41">
         <f t="shared" ref="G41:H41" si="8">A31</f>
@@ -1960,7 +1960,7 @@
     <row r="42" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F42">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G42">
         <f t="shared" ref="G42:H42" si="9">A32</f>

</xml_diff>

<commit_message>
P27 et P28 CSV
</commit_message>
<xml_diff>
--- a/Saison22/DonnéesCSV/Saisie des points.xlsx
+++ b/Saison22/DonnéesCSV/Saisie des points.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://054gc-my.sharepoint.com/personal/martin_sirois_statcan_gc_ca/Documents/01_Perso/GEHStatcan GIT/gehstatcan.github.io/Saison22/DonnéesCSV/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siromar\Documents\Github\gehstatcan.github.io\Saison22\DonnéesCSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="13_ncr:1_{2591EECF-29F7-4098-BC41-C06DE1DF147F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC6CC458-9C83-44C6-9894-B613ABAC8F36}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D762987-9A23-4CB0-9D35-BAE27A742FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1015,7 +1015,7 @@
   <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="K4" sqref="K4:K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,7 +1053,7 @@
         <v>138</v>
       </c>
       <c r="B2" s="3">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1061,11 +1061,11 @@
         <v>131</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <f>VLOOKUP(B3,tblÉquipes[[#All],[NomÉquipe]:[NoÉquipe2]],4,FALSE)</f>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>139</v>
@@ -1085,64 +1085,64 @@
         <v>132</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <f>VLOOKUP(B4,tblÉquipes[[#All],[NomÉquipe]:[NoÉquipe2]],4,FALSE)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F4" cm="1">
         <f t="array" ref="F4:I13">_xlfn._xlws.FILTER(F18:I42,I18:I42&gt;0)</f>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
       <c r="I4">
-        <v>125</v>
+        <v>145</v>
       </c>
       <c r="K4" t="str">
         <f>F4&amp;","&amp;G4&amp;","&amp;H4&amp;","&amp;I4</f>
-        <v>26,4,1,125</v>
+        <v>28,1,1,145</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F5">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H5">
         <v>2</v>
       </c>
       <c r="I5">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="K5" t="str">
         <f t="shared" ref="K5:K13" si="0">F5&amp;","&amp;G5&amp;","&amp;H5&amp;","&amp;I5</f>
-        <v>26,4,2,80</v>
+        <v>28,1,2,60</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F6">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I6">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="0"/>
-        <v>26,4,3,80</v>
+        <v>28,1,4,90</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1159,159 +1159,159 @@
         <v>137</v>
       </c>
       <c r="F7">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I7">
-        <v>85</v>
+        <v>20</v>
       </c>
       <c r="K7" t="str">
         <f t="shared" si="0"/>
-        <v>26,4,4,85</v>
+        <v>28,1,5,20</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" cm="1">
-        <f t="array" ref="A8:C26">_xlfn._xlws.FILTER(tblJoueurs!I:K,(tblJoueurs!I:I=$C$3)+(tblJoueurs!I:I=$C$4),"")</f>
-        <v>4</v>
+        <f t="array" ref="A8:C27">_xlfn._xlws.FILTER(tblJoueurs!I:K,(tblJoueurs!I:I=$C$3)+(tblJoueurs!I:I=$C$4),"")</f>
+        <v>1</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="str">
-        <v>Sébastien Landry</v>
+        <v>Kevin Borrelli</v>
       </c>
       <c r="D8" s="3">
-        <v>125</v>
+        <v>145</v>
       </c>
       <c r="F8">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H8">
         <v>99</v>
       </c>
       <c r="I8">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="0"/>
-        <v>26,4,99,45</v>
+        <v>28,1,99,35</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9" t="str">
-        <v>Frédéric Bédard</v>
+        <v>Claude Dionne</v>
       </c>
       <c r="D9" s="3">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="F9">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G9">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H9">
         <v>1</v>
       </c>
       <c r="I9">
-        <v>110</v>
+        <v>170</v>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="0"/>
-        <v>26,8,1,110</v>
+        <v>28,6,1,170</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B10">
         <v>3</v>
       </c>
       <c r="C10" t="str">
-        <v>Geneviève Ouellet</v>
-      </c>
-      <c r="D10" s="3">
-        <v>80</v>
-      </c>
+        <v>Bertrand Ouellet-Léveillé</v>
+      </c>
+      <c r="D10" s="3"/>
       <c r="F10">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G10">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H10">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I10">
-        <v>105</v>
+        <v>45</v>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="0"/>
-        <v>26,8,5,105</v>
+        <v>28,6,2,45</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B11">
         <v>4</v>
       </c>
       <c r="C11" t="str">
-        <v>Samuel Vézina</v>
+        <v>Bruno Morin</v>
       </c>
       <c r="D11" s="3">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F11">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G11">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H11">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I11">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" si="0"/>
-        <v>26,8,6,20</v>
+        <v>28,6,3,55</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B12">
         <v>5</v>
       </c>
       <c r="C12" t="str">
-        <v>Jean-Dominique Morency</v>
-      </c>
-      <c r="D12" s="3"/>
+        <v>François Lavoie</v>
+      </c>
+      <c r="D12" s="3">
+        <v>20</v>
+      </c>
       <c r="F12">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G12">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H12">
         <v>8</v>
@@ -1321,25 +1321,25 @@
       </c>
       <c r="K12" t="str">
         <f t="shared" si="0"/>
-        <v>26,8,8,20</v>
+        <v>28,6,8,20</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B13">
         <v>6</v>
       </c>
       <c r="C13" t="str">
-        <v>Stéphane Martineau</v>
+        <v>Étienne Lemyre (Disciples)</v>
       </c>
       <c r="D13" s="3"/>
       <c r="F13">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G13">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H13">
         <v>99</v>
@@ -1349,44 +1349,48 @@
       </c>
       <c r="K13" t="str">
         <f t="shared" si="0"/>
-        <v>26,8,99,55</v>
+        <v>28,6,99,55</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B14">
         <v>7</v>
       </c>
       <c r="C14" t="str">
-        <v>Michel Parenteau</v>
+        <v>Absent Absent</v>
       </c>
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B15">
-        <v>8</v>
+        <v>99</v>
       </c>
       <c r="C15" t="str">
-        <v>Caroline Pelletier</v>
-      </c>
-      <c r="D15" s="3"/>
+        <v>NA Les Disciples de Yaourt</v>
+      </c>
+      <c r="D15" s="3">
+        <v>35</v>
+      </c>
     </row>
     <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B16">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C16" t="str">
-        <v>Absent Absent</v>
-      </c>
-      <c r="D16" s="3"/>
+        <v>Stéphane Mongeau</v>
+      </c>
+      <c r="D16" s="3">
+        <v>170</v>
+      </c>
       <c r="F16" s="6" t="s">
         <v>141</v>
       </c>
@@ -1395,13 +1399,13 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B17">
-        <v>99</v>
+        <v>2</v>
       </c>
       <c r="C17" t="str">
-        <v>NA Les Herbizarres</v>
+        <v>Pierre-Olivier Julien</v>
       </c>
       <c r="D17" s="3">
         <v>45</v>
@@ -1421,24 +1425,24 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C18" t="str">
-        <v>Stéphanie Audet-Brazeau</v>
+        <v>Julien Bérard-Chagnon</v>
       </c>
       <c r="D18" s="3">
-        <v>110</v>
+        <v>55</v>
       </c>
       <c r="F18">
         <f>$B$2</f>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G18">
         <f t="shared" ref="G18:G38" si="1">A8</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H18">
         <f t="shared" ref="H18:H38" si="2">B8</f>
@@ -1446,27 +1450,27 @@
       </c>
       <c r="I18">
         <f t="shared" ref="I18:I38" si="3">D8</f>
-        <v>125</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C19" t="str">
-        <v>Julia Colpron</v>
+        <v>Patrick Charbonneau</v>
       </c>
       <c r="D19" s="3"/>
       <c r="F19">
         <f t="shared" ref="F19:F42" si="4">$B$2</f>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G19">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H19">
         <f t="shared" si="2"/>
@@ -1474,27 +1478,27 @@
       </c>
       <c r="I19">
         <f t="shared" si="3"/>
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B20">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C20" t="str">
-        <v>Isabelle Gamache</v>
+        <v>Keven Bosa</v>
       </c>
       <c r="D20" s="3"/>
       <c r="F20">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G20">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H20">
         <f t="shared" si="2"/>
@@ -1502,27 +1506,27 @@
       </c>
       <c r="I20">
         <f t="shared" si="3"/>
-        <v>80</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B21">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C21" t="str">
-        <v>Catherine Lachance</v>
+        <v>Étienne Rassart</v>
       </c>
       <c r="D21" s="3"/>
       <c r="F21">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G21">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H21">
         <f t="shared" si="2"/>
@@ -1530,29 +1534,27 @@
       </c>
       <c r="I21">
         <f t="shared" si="3"/>
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B22">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C22" t="str">
-        <v>Francis Vilandré</v>
-      </c>
-      <c r="D22" s="3">
-        <v>105</v>
-      </c>
+        <v>Daphné Allard Gervais</v>
+      </c>
+      <c r="D22" s="3"/>
       <c r="F22">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G22">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H22">
         <f t="shared" si="2"/>
@@ -1560,29 +1562,29 @@
       </c>
       <c r="I22">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
+        <v>6</v>
+      </c>
+      <c r="B23">
         <v>8</v>
       </c>
-      <c r="B23">
-        <v>6</v>
-      </c>
       <c r="C23" t="str">
-        <v>Julie Sarrazin</v>
+        <v>Emy Bourdages</v>
       </c>
       <c r="D23" s="3">
         <v>20</v>
       </c>
       <c r="F23">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G23">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H23">
         <f t="shared" si="2"/>
@@ -1595,22 +1597,22 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B24">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C24" t="str">
-        <v>Absent Absent</v>
+        <v>David Binet</v>
       </c>
       <c r="D24" s="3"/>
       <c r="F24">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G24">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H24">
         <f t="shared" si="2"/>
@@ -1623,77 +1625,84 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B25">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C25" t="str">
-        <v>Émilie Fougères</v>
-      </c>
-      <c r="D25" s="3">
-        <v>20</v>
-      </c>
+        <v>Absent Absent</v>
+      </c>
+      <c r="D25" s="3"/>
       <c r="F25">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G25">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H25">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>99</v>
       </c>
       <c r="I25">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B26">
-        <v>99</v>
+        <v>11</v>
       </c>
       <c r="C26" t="str">
-        <v>NA Les Génies de la traduction</v>
-      </c>
-      <c r="D26" s="3">
-        <v>55</v>
-      </c>
+        <v>François Sergerie</v>
+      </c>
+      <c r="D26" s="3"/>
       <c r="F26">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G26">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H26">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I26">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>170</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D27" s="3"/>
+      <c r="A27">
+        <v>6</v>
+      </c>
+      <c r="B27">
+        <v>99</v>
+      </c>
+      <c r="C27" t="str">
+        <v>NA Les 12e meilleurs</v>
+      </c>
+      <c r="D27" s="3">
+        <v>55</v>
+      </c>
       <c r="F27">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G27">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H27">
         <f t="shared" si="2"/>
-        <v>99</v>
+        <v>2</v>
       </c>
       <c r="I27">
         <f t="shared" si="3"/>
@@ -1704,34 +1713,34 @@
       <c r="D28" s="3"/>
       <c r="F28">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G28">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H28">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I28">
         <f t="shared" si="3"/>
-        <v>110</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D29" s="3"/>
       <c r="F29">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G29">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H29">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I29">
         <f t="shared" si="3"/>
@@ -1742,15 +1751,15 @@
       <c r="D30" s="3"/>
       <c r="F30">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G30">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H30">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I30">
         <f t="shared" si="3"/>
@@ -1761,15 +1770,15 @@
       <c r="D31" s="3"/>
       <c r="F31">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G31">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H31">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I31">
         <f t="shared" si="3"/>
@@ -1780,33 +1789,33 @@
       <c r="D32" s="3"/>
       <c r="F32">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G32">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H32">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I32">
         <f t="shared" si="3"/>
-        <v>105</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F33">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G33">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H33">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I33">
         <f t="shared" si="3"/>
@@ -1816,15 +1825,15 @@
     <row r="34" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F34">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G34">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H34">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I34">
         <f t="shared" si="3"/>
@@ -1834,61 +1843,61 @@
     <row r="35" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F35">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G35">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H35">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I35">
         <f t="shared" si="3"/>
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F36">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G36">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H36">
         <f t="shared" si="2"/>
-        <v>99</v>
+        <v>11</v>
       </c>
       <c r="I36">
         <f t="shared" si="3"/>
-        <v>55</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F37">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G37">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H37">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="I37">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F38">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G38">
         <f t="shared" si="1"/>
@@ -1906,7 +1915,7 @@
     <row r="39" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F39">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G39">
         <f t="shared" ref="G39:H39" si="5">A29</f>
@@ -1924,7 +1933,7 @@
     <row r="40" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F40">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G40">
         <f t="shared" ref="G40:H40" si="7">A30</f>
@@ -1942,7 +1951,7 @@
     <row r="41" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F41">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G41">
         <f t="shared" ref="G41:H41" si="8">A31</f>
@@ -1960,7 +1969,7 @@
     <row r="42" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F42">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G42">
         <f t="shared" ref="G42:H42" si="9">A32</f>

</xml_diff>

<commit_message>
P41 et P42 CSV
</commit_message>
<xml_diff>
--- a/Saison22/DonnéesCSV/Saisie des points.xlsx
+++ b/Saison22/DonnéesCSV/Saisie des points.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\gehstatcan.github.io\Saison22\DonnéesCSV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siromar\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{051964F9-C09D-4903-966E-9ED66CA3DFF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Saisie" sheetId="1" r:id="rId1"/>
     <sheet name="tblÉquipes" sheetId="3" r:id="rId2"/>
     <sheet name="tblJoueurs" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,14 +38,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -526,7 +527,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -632,7 +633,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Sortie" xfId="1" builtinId="21"/>
+    <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
   <dxfs count="10">
     <dxf>
@@ -679,14 +680,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tblÉquipes" displayName="tblÉquipes" ref="A1:E9" totalsRowShown="0">
-  <autoFilter ref="A1:E9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="tblÉquipes" displayName="tblÉquipes" ref="A1:E9" totalsRowShown="0">
+  <autoFilter ref="A1:E9" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="NoÉquipe"/>
-    <tableColumn id="2" name="NomÉquipe" dataDxfId="9"/>
-    <tableColumn id="3" name="PosFinale" dataDxfId="8"/>
-    <tableColumn id="4" name="Carillon"/>
-    <tableColumn id="5" name="NoÉquipe2" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="NoÉquipe"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="NomÉquipe" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="PosFinale" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Carillon"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="NoÉquipe2" dataDxfId="7">
       <calculatedColumnFormula>tblÉquipes[[#This Row],[NoÉquipe]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -695,24 +696,24 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="tblJoueurs" displayName="tblJoueurs" ref="A1:K81" totalsRowShown="0">
-  <autoFilter ref="A1:K81"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="tblJoueurs" displayName="tblJoueurs" ref="A1:K81" totalsRowShown="0">
+  <autoFilter ref="A1:K81" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="11">
-    <tableColumn id="1" name="NoÉquipe"/>
-    <tableColumn id="2" name="NoJoueur"/>
-    <tableColumn id="3" name="NomJoueur" dataDxfId="6"/>
-    <tableColumn id="4" name="PrénomJoueur" dataDxfId="5"/>
-    <tableColumn id="5" name="Alias" dataDxfId="4"/>
-    <tableColumn id="6" name="Statut" dataDxfId="3"/>
-    <tableColumn id="7" name="Icône"/>
-    <tableColumn id="8" name="PosActuelle"/>
-    <tableColumn id="11" name="NoÉquipe2" dataDxfId="2">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="NoÉquipe"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="NoJoueur"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="NomJoueur" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="PrénomJoueur" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Alias" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Statut" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Icône"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="PosActuelle"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="NoÉquipe2" dataDxfId="2">
       <calculatedColumnFormula>tblJoueurs[[#This Row],[NoÉquipe]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="NoJoueur2" dataDxfId="1">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="NoJoueur2" dataDxfId="1">
       <calculatedColumnFormula>tblJoueurs[[#This Row],[NoJoueur]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Nom complet" dataDxfId="0">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Nom complet" dataDxfId="0">
       <calculatedColumnFormula>tblJoueurs[[#This Row],[PrénomJoueur]] &amp; " " &amp;tblJoueurs[[#This Row],[NomJoueur]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1016,14 +1017,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4:K13"/>
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
@@ -1058,7 +1059,7 @@
         <v>138</v>
       </c>
       <c r="B2" s="3">
-        <v>28</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1066,11 +1067,11 @@
         <v>131</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <f>VLOOKUP(B3,tblÉquipes[[#All],[NomÉquipe]:[NoÉquipe2]],4,FALSE)</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>139</v>
@@ -1096,69 +1097,58 @@
         <f>VLOOKUP(B4,tblÉquipes[[#All],[NomÉquipe]:[NoÉquipe2]],4,FALSE)</f>
         <v>6</v>
       </c>
-      <c r="F4" t="e" cm="1">
-        <f t="array" aca="1" ref="F4:I13" ca="1">_xlfn._xlws.FILTER(F18:I42,I18:I42&gt;0)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="G4" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="H4" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="I4" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="K4" t="e">
-        <f ca="1">F4&amp;","&amp;G4&amp;","&amp;H4&amp;","&amp;I4</f>
-        <v>#NAME?</v>
+      <c r="F4" cm="1">
+        <f t="array" ref="F4:I13">_xlfn._xlws.FILTER(F18:I45,I18:I45&gt;0)</f>
+        <v>42</v>
+      </c>
+      <c r="G4">
+        <v>6</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>100</v>
+      </c>
+      <c r="K4" t="str">
+        <f>F4&amp;","&amp;G4&amp;","&amp;H4&amp;","&amp;I4</f>
+        <v>42,6,1,100</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F5" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="G5" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="H5" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="I5" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="K5" t="e">
-        <f t="shared" ref="K5:K13" ca="1" si="0">F5&amp;","&amp;G5&amp;","&amp;H5&amp;","&amp;I5</f>
-        <v>#NAME?</v>
+      <c r="F5">
+        <v>42</v>
+      </c>
+      <c r="G5">
+        <v>6</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>40</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" ref="K5:K13" si="0">F5&amp;","&amp;G5&amp;","&amp;H5&amp;","&amp;I5</f>
+        <v>42,6,2,40</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F6" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="G6" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="H6" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="I6" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="K6" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
+      <c r="F6">
+        <v>42</v>
+      </c>
+      <c r="G6">
+        <v>6</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>180</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="0"/>
+        <v>42,6,4,180</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1174,292 +1164,234 @@
       <c r="D7" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="F7" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="G7" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="H7" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="I7" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="K7" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
+      <c r="F7">
+        <v>42</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="H7">
+        <v>9</v>
+      </c>
+      <c r="I7">
+        <v>30</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="0"/>
+        <v>42,6,9,30</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="e" cm="1">
-        <f t="array" aca="1" ref="A8:C27" ca="1">_xlfn._xlws.FILTER(tblJoueurs!I:K,(tblJoueurs!I:I=$C$3)+(tblJoueurs!I:I=$C$4),"")</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="B8" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="C8" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+      <c r="A8" cm="1">
+        <f t="array" ref="A8:C33">_xlfn._xlws.FILTER(tblJoueurs!I:K,(tblJoueurs!I:I=$C$3)+(tblJoueurs!I:I=$C$4),"")</f>
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Stéphane Mongeau</v>
       </c>
       <c r="D8" s="3">
-        <v>145</v>
-      </c>
-      <c r="F8" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="G8" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="H8" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="I8" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="K8" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
+        <v>100</v>
+      </c>
+      <c r="F8">
+        <v>42</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
+      </c>
+      <c r="H8">
+        <v>99</v>
+      </c>
+      <c r="I8">
+        <v>55</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="0"/>
+        <v>42,6,99,55</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="B9" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="C9" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="str">
+        <v>Pierre-Olivier Julien</v>
       </c>
       <c r="D9" s="3">
-        <v>60</v>
-      </c>
-      <c r="F9" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="G9" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="H9" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="I9" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="K9" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
+        <v>40</v>
+      </c>
+      <c r="F9">
+        <v>42</v>
+      </c>
+      <c r="G9">
+        <v>7</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>75</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="0"/>
+        <v>42,7,1,75</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="B10" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="C10" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Julien Bérard-Chagnon</v>
       </c>
       <c r="D10" s="3"/>
-      <c r="F10" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="G10" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="H10" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="I10" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="K10" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
+      <c r="F10">
+        <v>42</v>
+      </c>
+      <c r="G10">
+        <v>7</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+      <c r="I10">
+        <v>50</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="0"/>
+        <v>42,7,2,50</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="B11" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="C11" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11" t="str">
+        <v>Patrick Charbonneau</v>
       </c>
       <c r="D11" s="3">
-        <v>90</v>
-      </c>
-      <c r="F11" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="G11" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="H11" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="I11" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="K11" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
+        <v>180</v>
+      </c>
+      <c r="F11">
+        <v>42</v>
+      </c>
+      <c r="G11">
+        <v>7</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="I11">
+        <v>40</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="0"/>
+        <v>42,7,3,40</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="B12" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="C12" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="D12" s="3">
-        <v>20</v>
-      </c>
-      <c r="F12" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="G12" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="H12" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="I12" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="K12" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12" t="str">
+        <v>Keven Bosa</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="F12">
+        <v>42</v>
+      </c>
+      <c r="G12">
+        <v>7</v>
+      </c>
+      <c r="H12">
+        <v>4</v>
+      </c>
+      <c r="I12">
+        <v>50</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="0"/>
+        <v>42,7,4,50</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="B13" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="C13" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Étienne Rassart</v>
       </c>
       <c r="D13" s="3"/>
-      <c r="F13" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="G13" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="H13" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="I13" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="K13" t="e">
-        <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
+      <c r="F13">
+        <v>42</v>
+      </c>
+      <c r="G13">
+        <v>7</v>
+      </c>
+      <c r="H13">
+        <v>99</v>
+      </c>
+      <c r="I13">
+        <v>40</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="0"/>
+        <v>42,7,99,40</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="B14" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="C14" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <v>7</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Daphné Allard Gervais</v>
       </c>
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="B15" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="C15" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="D15" s="3">
-        <v>35</v>
-      </c>
+      <c r="A15">
+        <v>6</v>
+      </c>
+      <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="C15" t="str">
+        <v>Emy Bourdages</v>
+      </c>
+      <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="B16" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="C16" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+      <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16">
+        <v>9</v>
+      </c>
+      <c r="C16" t="str">
+        <v>David Binet</v>
       </c>
       <c r="D16" s="3">
-        <v>170</v>
+        <v>30</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>141</v>
@@ -1468,21 +1400,16 @@
       <c r="H16" s="6"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="B17" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="C17" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="D17" s="3">
-        <v>45</v>
-      </c>
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17" t="str">
+        <v>Absent Absent</v>
+      </c>
+      <c r="D17" s="3"/>
       <c r="F17" s="2" t="s">
         <v>139</v>
       </c>
@@ -1497,94 +1424,85 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="B18" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="C18" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="D18" s="3">
-        <v>55</v>
-      </c>
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="B18">
+        <v>11</v>
+      </c>
+      <c r="C18" t="str">
+        <v>François Sergerie</v>
+      </c>
+      <c r="D18" s="3"/>
       <c r="F18">
         <f>$B$2</f>
-        <v>28</v>
-      </c>
-      <c r="G18" t="e">
-        <f t="shared" ref="G18:G38" ca="1" si="1">A8</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="H18" t="e">
-        <f t="shared" ref="H18:H38" ca="1" si="2">B8</f>
-        <v>#NAME?</v>
+        <v>42</v>
+      </c>
+      <c r="G18">
+        <f t="shared" ref="G18:G38" si="1">A8</f>
+        <v>6</v>
+      </c>
+      <c r="H18">
+        <f t="shared" ref="H18:H38" si="2">B8</f>
+        <v>1</v>
       </c>
       <c r="I18">
         <f t="shared" ref="I18:I38" si="3">D8</f>
-        <v>145</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="B19" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="C19" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <v>12</v>
+      </c>
+      <c r="C19" t="str">
+        <v>Arnaud Bouchard-Santerre</v>
       </c>
       <c r="D19" s="3"/>
       <c r="F19">
-        <f t="shared" ref="F19:F42" si="4">$B$2</f>
-        <v>28</v>
-      </c>
-      <c r="G19" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="H19" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NAME?</v>
+        <f t="shared" ref="F19:F45" si="4">$B$2</f>
+        <v>42</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="I19">
         <f t="shared" si="3"/>
-        <v>60</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="B20" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="C20" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="D20" s="3"/>
+      <c r="A20">
+        <v>6</v>
+      </c>
+      <c r="B20">
+        <v>99</v>
+      </c>
+      <c r="C20" t="str">
+        <v>NA Les 12e meilleurs</v>
+      </c>
+      <c r="D20" s="3">
+        <v>55</v>
+      </c>
       <c r="F20">
         <f t="shared" si="4"/>
-        <v>28</v>
-      </c>
-      <c r="G20" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="H20" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NAME?</v>
+        <v>42</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="2"/>
+        <v>3</v>
       </c>
       <c r="I20">
         <f t="shared" si="3"/>
@@ -1592,94 +1510,89 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="B21" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="C21" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="D21" s="3"/>
+      <c r="A21">
+        <v>7</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="str">
+        <v>Philippe Bérubé</v>
+      </c>
+      <c r="D21" s="3">
+        <v>75</v>
+      </c>
       <c r="F21">
         <f t="shared" si="4"/>
-        <v>28</v>
-      </c>
-      <c r="G21" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="H21" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NAME?</v>
+        <v>42</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="I21">
         <f t="shared" si="3"/>
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="B22" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="C22" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="D22" s="3"/>
+      <c r="A22">
+        <v>7</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22" t="str">
+        <v>Tony Labillois</v>
+      </c>
+      <c r="D22" s="3">
+        <v>50</v>
+      </c>
       <c r="F22">
         <f t="shared" si="4"/>
-        <v>28</v>
-      </c>
-      <c r="G22" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="H22" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NAME?</v>
+        <v>42</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="I22">
         <f t="shared" si="3"/>
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="B23" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="C23" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+      <c r="A23">
+        <v>7</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23" t="str">
+        <v>Éric Caron-Malenfant</v>
       </c>
       <c r="D23" s="3">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="F23">
         <f t="shared" si="4"/>
-        <v>28</v>
-      </c>
-      <c r="G23" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="H23" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NAME?</v>
+        <v>42</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="2"/>
+        <v>6</v>
       </c>
       <c r="I23">
         <f t="shared" si="3"/>
@@ -1687,30 +1600,29 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="B24" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="C24" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="D24" s="3"/>
+      <c r="A24">
+        <v>7</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24" t="str">
+        <v>Pierre Galarneau</v>
+      </c>
+      <c r="D24" s="3">
+        <v>50</v>
+      </c>
       <c r="F24">
         <f t="shared" si="4"/>
-        <v>28</v>
-      </c>
-      <c r="G24" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="H24" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NAME?</v>
+        <v>42</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="2"/>
+        <v>7</v>
       </c>
       <c r="I24">
         <f t="shared" si="3"/>
@@ -1718,132 +1630,139 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="B25" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="C25" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+      <c r="A25">
+        <v>7</v>
+      </c>
+      <c r="B25">
+        <v>5</v>
+      </c>
+      <c r="C25" t="str">
+        <v>Félix Labrecque-Synnott</v>
       </c>
       <c r="D25" s="3"/>
       <c r="F25">
         <f t="shared" si="4"/>
-        <v>28</v>
-      </c>
-      <c r="G25" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="H25" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NAME?</v>
+        <v>42</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="I25">
         <f t="shared" si="3"/>
-        <v>35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="B26" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="C26" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+      <c r="A26">
+        <v>7</v>
+      </c>
+      <c r="B26">
+        <v>6</v>
+      </c>
+      <c r="C26" t="str">
+        <v>Danielle Turpin</v>
       </c>
       <c r="D26" s="3"/>
       <c r="F26">
         <f t="shared" si="4"/>
-        <v>28</v>
-      </c>
-      <c r="G26" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="H26" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NAME?</v>
+        <v>42</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
       <c r="I26">
         <f t="shared" si="3"/>
-        <v>170</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="B27" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="C27" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="D27" s="3">
-        <v>55</v>
-      </c>
+      <c r="A27">
+        <v>7</v>
+      </c>
+      <c r="B27">
+        <v>7</v>
+      </c>
+      <c r="C27" t="str">
+        <v>James Falconer</v>
+      </c>
+      <c r="D27" s="3"/>
       <c r="F27">
         <f t="shared" si="4"/>
-        <v>28</v>
-      </c>
-      <c r="G27" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="H27" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NAME?</v>
+        <v>42</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
       <c r="I27">
         <f t="shared" si="3"/>
-        <v>45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>7</v>
+      </c>
+      <c r="B28">
+        <v>8</v>
+      </c>
+      <c r="C28" t="str">
+        <v>Absent Absent</v>
+      </c>
       <c r="D28" s="3"/>
       <c r="F28">
         <f t="shared" si="4"/>
-        <v>28</v>
-      </c>
-      <c r="G28" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="H28" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NAME?</v>
+        <v>42</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="I28">
         <f t="shared" si="3"/>
-        <v>55</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>7</v>
+      </c>
+      <c r="B29">
+        <v>9</v>
+      </c>
+      <c r="C29" t="str">
+        <v>Catherine NA</v>
+      </c>
       <c r="D29" s="3"/>
       <c r="F29">
         <f t="shared" si="4"/>
-        <v>28</v>
-      </c>
-      <c r="G29" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="H29" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NAME?</v>
+        <v>42</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="2"/>
+        <v>12</v>
       </c>
       <c r="I29">
         <f t="shared" si="3"/>
@@ -1851,239 +1770,332 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>7</v>
+      </c>
+      <c r="B30">
+        <v>10</v>
+      </c>
+      <c r="C30" t="str">
+        <v>Louis NA</v>
+      </c>
       <c r="D30" s="3"/>
       <c r="F30">
         <f t="shared" si="4"/>
-        <v>28</v>
-      </c>
-      <c r="G30" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="H30" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NAME?</v>
+        <v>42</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="2"/>
+        <v>99</v>
       </c>
       <c r="I30">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>7</v>
+      </c>
+      <c r="B31">
+        <v>11</v>
+      </c>
+      <c r="C31" t="str">
+        <v>Étienne Lemyre (Faciles)</v>
+      </c>
       <c r="D31" s="3"/>
       <c r="F31">
         <f t="shared" si="4"/>
-        <v>28</v>
-      </c>
-      <c r="G31" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="H31" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NAME?</v>
+        <v>42</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="I31">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>7</v>
+      </c>
+      <c r="B32">
+        <v>12</v>
+      </c>
+      <c r="C32" t="str">
+        <v>Élizabeth LeBlanc</v>
+      </c>
       <c r="D32" s="3"/>
       <c r="F32">
         <f t="shared" si="4"/>
-        <v>28</v>
-      </c>
-      <c r="G32" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="H32" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NAME?</v>
+        <v>42</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="I32">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="6:9" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>7</v>
+      </c>
+      <c r="B33">
+        <v>99</v>
+      </c>
+      <c r="C33" t="str">
+        <v>NA Les Faciles à cuire</v>
+      </c>
+      <c r="D33" s="3">
+        <v>40</v>
+      </c>
       <c r="F33">
         <f t="shared" si="4"/>
-        <v>28</v>
-      </c>
-      <c r="G33" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="H33" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NAME?</v>
+        <v>42</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="2"/>
+        <v>3</v>
       </c>
       <c r="I33">
         <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="6:9" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F34">
         <f t="shared" si="4"/>
-        <v>28</v>
-      </c>
-      <c r="G34" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="H34" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NAME?</v>
+        <v>42</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="I34">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="6:9" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F35">
         <f t="shared" si="4"/>
-        <v>28</v>
-      </c>
-      <c r="G35" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="H35" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NAME?</v>
+        <v>42</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="I35">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F36">
         <f t="shared" si="4"/>
-        <v>28</v>
-      </c>
-      <c r="G36" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="H36" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NAME?</v>
+        <v>42</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="2"/>
+        <v>6</v>
       </c>
       <c r="I36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F37">
         <f t="shared" si="4"/>
-        <v>28</v>
-      </c>
-      <c r="G37" t="e">
-        <f t="shared" ca="1" si="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="H37" t="e">
-        <f t="shared" ca="1" si="2"/>
-        <v>#NAME?</v>
+        <v>42</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="2"/>
+        <v>7</v>
       </c>
       <c r="I37">
         <f t="shared" si="3"/>
-        <v>55</v>
-      </c>
-    </row>
-    <row r="38" spans="6:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F38">
         <f t="shared" si="4"/>
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="G38">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H38">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I38">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F39">
         <f t="shared" si="4"/>
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="G39">
         <f t="shared" ref="G39:H39" si="5">A29</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H39">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="I39">
         <f t="shared" ref="I39:I42" si="6">D29</f>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F40">
         <f t="shared" si="4"/>
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="G40">
         <f t="shared" ref="G40:H40" si="7">A30</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H40">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I40">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F41">
         <f t="shared" si="4"/>
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="G41">
         <f t="shared" ref="G41:H41" si="8">A31</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H41">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="I41">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F42">
         <f t="shared" si="4"/>
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="G42">
         <f t="shared" ref="G42:H42" si="9">A32</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H42">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I42">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <f t="shared" si="4"/>
+        <v>42</v>
+      </c>
+      <c r="G43">
+        <f t="shared" ref="G43:G45" si="10">A33</f>
+        <v>7</v>
+      </c>
+      <c r="H43">
+        <f t="shared" ref="H43:H45" si="11">B33</f>
+        <v>99</v>
+      </c>
+      <c r="I43">
+        <f t="shared" ref="I43:I45" si="12">D33</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <f t="shared" si="4"/>
+        <v>42</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <f t="shared" si="4"/>
+        <v>42</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -2096,8 +2108,8 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>tblÉquipes!$B$2:$B$9</xm:f>
           </x14:formula1>
@@ -2110,14 +2122,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
@@ -2296,12 +2308,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q81"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
@@ -3085,17 +3097,15 @@
         <f>tblJoueurs[[#This Row],[PrénomJoueur]] &amp; " " &amp;tblJoueurs[[#This Row],[NomJoueur]]</f>
         <v>NA Les Bons Perdants</v>
       </c>
-      <c r="M18" t="e" cm="1">
-        <f t="array" aca="1" ref="M18:O25" ca="1">_xlfn._xlws.FILTER(J:L,I:I=1)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="N18" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="O18" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+      <c r="M18" cm="1">
+        <f t="array" ref="M18:O25">_xlfn._xlws.FILTER(J:L,I:I=1)</f>
+        <v>1</v>
+      </c>
+      <c r="N18" t="str">
+        <v>Kevin Borrelli</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -3135,17 +3145,14 @@
         <f>tblJoueurs[[#This Row],[PrénomJoueur]] &amp; " " &amp;tblJoueurs[[#This Row],[NomJoueur]]</f>
         <v>Mark Switzer</v>
       </c>
-      <c r="M19" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="N19" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="O19" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+      <c r="M19">
+        <v>2</v>
+      </c>
+      <c r="N19" t="str">
+        <v>Claude Dionne</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
@@ -3185,17 +3192,14 @@
         <f>tblJoueurs[[#This Row],[PrénomJoueur]] &amp; " " &amp;tblJoueurs[[#This Row],[NomJoueur]]</f>
         <v>Pierre Parent</v>
       </c>
-      <c r="M20" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="N20" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="O20" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+      <c r="M20">
+        <v>3</v>
+      </c>
+      <c r="N20" t="str">
+        <v>Bertrand Ouellet-Léveillé</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -3235,17 +3239,14 @@
         <f>tblJoueurs[[#This Row],[PrénomJoueur]] &amp; " " &amp;tblJoueurs[[#This Row],[NomJoueur]]</f>
         <v>François Rivest</v>
       </c>
-      <c r="M21" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="N21" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="O21" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+      <c r="M21">
+        <v>4</v>
+      </c>
+      <c r="N21" t="str">
+        <v>Bruno Morin</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -3285,17 +3286,14 @@
         <f>tblJoueurs[[#This Row],[PrénomJoueur]] &amp; " " &amp;tblJoueurs[[#This Row],[NomJoueur]]</f>
         <v>André Delage</v>
       </c>
-      <c r="M22" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="N22" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="O22" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+      <c r="M22">
+        <v>5</v>
+      </c>
+      <c r="N22" t="str">
+        <v>François Lavoie</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -3335,17 +3333,14 @@
         <f>tblJoueurs[[#This Row],[PrénomJoueur]] &amp; " " &amp;tblJoueurs[[#This Row],[NomJoueur]]</f>
         <v>Louise Maheux</v>
       </c>
-      <c r="M23" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="N23" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="O23" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+      <c r="M23">
+        <v>6</v>
+      </c>
+      <c r="N23" t="str">
+        <v>Étienne Lemyre (Disciples)</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -3385,17 +3380,14 @@
         <f>tblJoueurs[[#This Row],[PrénomJoueur]] &amp; " " &amp;tblJoueurs[[#This Row],[NomJoueur]]</f>
         <v>Yanick Aubé</v>
       </c>
-      <c r="M24" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="N24" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="O24" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+      <c r="M24">
+        <v>7</v>
+      </c>
+      <c r="N24" t="str">
+        <v>Absent Absent</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -3435,17 +3427,14 @@
         <f>tblJoueurs[[#This Row],[PrénomJoueur]] &amp; " " &amp;tblJoueurs[[#This Row],[NomJoueur]]</f>
         <v>Jean-Michel M.</v>
       </c>
-      <c r="M25" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="N25" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="O25" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+      <c r="M25">
+        <v>99</v>
+      </c>
+      <c r="N25" t="str">
+        <v>NA Les Disciples de Yaourt</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
P47, correction Samuel B.
</commit_message>
<xml_diff>
--- a/Saison22/DonnéesCSV/Saisie des points.xlsx
+++ b/Saison22/DonnéesCSV/Saisie des points.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siromar\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://054gc-my.sharepoint.com/personal/martin_sirois_statcan_gc_ca/Documents/01_Perso/GEHStatcan GIT/gehstatcan.github.io/gehstatcan.github.io/Saison22/DonnéesCSV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{051964F9-C09D-4903-966E-9ED66CA3DFF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="13_ncr:1_{051964F9-C09D-4903-966E-9ED66CA3DFF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D7E13AC-D576-4EDA-B412-A645ED85165B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -1021,7 +1021,7 @@
   <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1059,7 +1059,7 @@
         <v>138</v>
       </c>
       <c r="B2" s="3">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1099,7 +1099,7 @@
       </c>
       <c r="F4" cm="1">
         <f t="array" ref="F4:I13">_xlfn._xlws.FILTER(F18:I45,I18:I45&gt;0)</f>
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G4">
         <v>6</v>
@@ -1112,12 +1112,12 @@
       </c>
       <c r="K4" t="str">
         <f>F4&amp;","&amp;G4&amp;","&amp;H4&amp;","&amp;I4</f>
-        <v>42,6,1,100</v>
+        <v>47,6,1,100</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F5">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G5">
         <v>6</v>
@@ -1130,12 +1130,12 @@
       </c>
       <c r="K5" t="str">
         <f t="shared" ref="K5:K13" si="0">F5&amp;","&amp;G5&amp;","&amp;H5&amp;","&amp;I5</f>
-        <v>42,6,2,40</v>
+        <v>47,6,2,40</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F6">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G6">
         <v>6</v>
@@ -1148,7 +1148,7 @@
       </c>
       <c r="K6" t="str">
         <f t="shared" si="0"/>
-        <v>42,6,4,180</v>
+        <v>47,6,4,180</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1165,7 +1165,7 @@
         <v>137</v>
       </c>
       <c r="F7">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G7">
         <v>6</v>
@@ -1178,7 +1178,7 @@
       </c>
       <c r="K7" t="str">
         <f t="shared" si="0"/>
-        <v>42,6,9,30</v>
+        <v>47,6,9,30</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1196,7 +1196,7 @@
         <v>100</v>
       </c>
       <c r="F8">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G8">
         <v>6</v>
@@ -1209,7 +1209,7 @@
       </c>
       <c r="K8" t="str">
         <f t="shared" si="0"/>
-        <v>42,6,99,55</v>
+        <v>47,6,99,55</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1226,7 +1226,7 @@
         <v>40</v>
       </c>
       <c r="F9">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G9">
         <v>7</v>
@@ -1239,7 +1239,7 @@
       </c>
       <c r="K9" t="str">
         <f t="shared" si="0"/>
-        <v>42,7,1,75</v>
+        <v>47,7,1,75</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1254,7 +1254,7 @@
       </c>
       <c r="D10" s="3"/>
       <c r="F10">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G10">
         <v>7</v>
@@ -1267,7 +1267,7 @@
       </c>
       <c r="K10" t="str">
         <f t="shared" si="0"/>
-        <v>42,7,2,50</v>
+        <v>47,7,2,50</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1284,7 +1284,7 @@
         <v>180</v>
       </c>
       <c r="F11">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G11">
         <v>7</v>
@@ -1297,7 +1297,7 @@
       </c>
       <c r="K11" t="str">
         <f t="shared" si="0"/>
-        <v>42,7,3,40</v>
+        <v>47,7,3,40</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1312,7 +1312,7 @@
       </c>
       <c r="D12" s="3"/>
       <c r="F12">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G12">
         <v>7</v>
@@ -1325,7 +1325,7 @@
       </c>
       <c r="K12" t="str">
         <f t="shared" si="0"/>
-        <v>42,7,4,50</v>
+        <v>47,7,4,50</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1340,7 +1340,7 @@
       </c>
       <c r="D13" s="3"/>
       <c r="F13">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G13">
         <v>7</v>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="K13" t="str">
         <f t="shared" si="0"/>
-        <v>42,7,99,40</v>
+        <v>47,7,99,40</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1436,7 +1436,7 @@
       <c r="D18" s="3"/>
       <c r="F18">
         <f>$B$2</f>
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G18">
         <f t="shared" ref="G18:G38" si="1">A8</f>
@@ -1464,7 +1464,7 @@
       <c r="D19" s="3"/>
       <c r="F19">
         <f t="shared" ref="F19:F45" si="4">$B$2</f>
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G19">
         <f t="shared" si="1"/>
@@ -1494,7 +1494,7 @@
       </c>
       <c r="F20">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G20">
         <f t="shared" si="1"/>
@@ -1524,7 +1524,7 @@
       </c>
       <c r="F21">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G21">
         <f t="shared" si="1"/>
@@ -1554,7 +1554,7 @@
       </c>
       <c r="F22">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G22">
         <f t="shared" si="1"/>
@@ -1584,7 +1584,7 @@
       </c>
       <c r="F23">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G23">
         <f t="shared" si="1"/>
@@ -1614,7 +1614,7 @@
       </c>
       <c r="F24">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G24">
         <f t="shared" si="1"/>
@@ -1642,7 +1642,7 @@
       <c r="D25" s="3"/>
       <c r="F25">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G25">
         <f t="shared" si="1"/>
@@ -1670,7 +1670,7 @@
       <c r="D26" s="3"/>
       <c r="F26">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G26">
         <f t="shared" si="1"/>
@@ -1698,7 +1698,7 @@
       <c r="D27" s="3"/>
       <c r="F27">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G27">
         <f t="shared" si="1"/>
@@ -1726,7 +1726,7 @@
       <c r="D28" s="3"/>
       <c r="F28">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G28">
         <f t="shared" si="1"/>
@@ -1754,7 +1754,7 @@
       <c r="D29" s="3"/>
       <c r="F29">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G29">
         <f t="shared" si="1"/>
@@ -1782,7 +1782,7 @@
       <c r="D30" s="3"/>
       <c r="F30">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G30">
         <f t="shared" si="1"/>
@@ -1810,7 +1810,7 @@
       <c r="D31" s="3"/>
       <c r="F31">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G31">
         <f t="shared" si="1"/>
@@ -1838,7 +1838,7 @@
       <c r="D32" s="3"/>
       <c r="F32">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G32">
         <f t="shared" si="1"/>
@@ -1868,7 +1868,7 @@
       </c>
       <c r="F33">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G33">
         <f t="shared" si="1"/>
@@ -1886,7 +1886,7 @@
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F34">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G34">
         <f t="shared" si="1"/>
@@ -1904,7 +1904,7 @@
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F35">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G35">
         <f t="shared" si="1"/>
@@ -1922,7 +1922,7 @@
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F36">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G36">
         <f t="shared" si="1"/>
@@ -1940,7 +1940,7 @@
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F37">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G37">
         <f t="shared" si="1"/>
@@ -1958,7 +1958,7 @@
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F38">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G38">
         <f t="shared" si="1"/>
@@ -1976,7 +1976,7 @@
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F39">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G39">
         <f t="shared" ref="G39:H39" si="5">A29</f>
@@ -1994,7 +1994,7 @@
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F40">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G40">
         <f t="shared" ref="G40:H40" si="7">A30</f>
@@ -2012,7 +2012,7 @@
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F41">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G41">
         <f t="shared" ref="G41:H41" si="8">A31</f>
@@ -2030,7 +2030,7 @@
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F42">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G42">
         <f t="shared" ref="G42:H42" si="9">A32</f>
@@ -2048,7 +2048,7 @@
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F43">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G43">
         <f t="shared" ref="G43:G45" si="10">A33</f>
@@ -2066,7 +2066,7 @@
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F44">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G44">
         <f t="shared" si="10"/>
@@ -2084,7 +2084,7 @@
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F45">
         <f t="shared" si="4"/>
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G45">
         <f t="shared" si="10"/>
@@ -2108,7 +2108,7 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>tblÉquipes!$B$2:$B$9</xm:f>

</xml_diff>